<commit_message>
Add all actions for auto mode in table
</commit_message>
<xml_diff>
--- a/recipes/test3.xlsx
+++ b/recipes/test3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,14 +466,10 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Act 4</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>F_2</t>
-        </is>
-      </c>
+          <t>Закрыть клапан насоса</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -484,21 +480,73 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Close valve</t>
+          <t>Открыть клапан</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ar</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>sdfsdfsd</t>
-        </is>
-      </c>
+          <t>C_2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Значение на РРГ с паузой</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>N_2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0030:02</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>kuda ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Стабилизировать давление</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1e-4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0000:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ewrr</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>